<commit_message>
fix defense and grade
</commit_message>
<xml_diff>
--- a/src/main/resources/template/excel/middleCheckForm.xlsx
+++ b/src/main/resources/template/excel/middleCheckForm.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>{{qrCode}}</t>
   </si>
@@ -200,72 +200,8 @@
     <t xml:space="preserve">{{majorAgree}} </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>教研室主任</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Tahoma"/>
-        <charset val="0"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>签名</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Tahoma"/>
-        <charset val="0"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Tahoma"/>
-        <charset val="0"/>
-      </rPr>
-      <t>{{majorSign}}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>日期：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Tahoma"/>
-        <charset val="0"/>
-      </rPr>
-      <t>{{majorDate}}</t>
-    </r>
+    <t>教研室主任(签名)：{{majorSign}}
+日期：{{majorDate}}</t>
   </si>
   <si>
     <t>学院意见</t>
@@ -274,72 +210,8 @@
     <t>{{collegeAgree}}</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>教学院长</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Tahoma"/>
-        <charset val="0"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>签名</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Tahoma"/>
-        <charset val="0"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Tahoma"/>
-        <charset val="0"/>
-      </rPr>
-      <t>{{collegeSign}}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="0"/>
-      </rPr>
-      <t>日期：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Tahoma"/>
-        <charset val="0"/>
-      </rPr>
-      <t>{{collegeDate}}</t>
-    </r>
+    <t>教学院长(签名)：{{collegeSign}}
+日期：{{collegeDate}}</t>
   </si>
 </sst>
 </file>
@@ -732,7 +604,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -809,33 +681,18 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -850,6 +707,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -867,37 +750,6 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1009,7 +861,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1039,7 +891,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1057,28 +909,28 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1087,10 +939,10 @@
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1148,7 +1000,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1189,35 +1041,26 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1569,8 +1412,8 @@
   <sheetPr/>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -1783,52 +1626,48 @@
       <c r="B13" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" ht="33" customHeight="1" spans="1:7">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" ht="33" customHeight="1" spans="1:7">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" ht="33" customHeight="1" spans="1:7">
       <c r="A16" s="13"/>
       <c r="B16" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
+        <v>49</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" ht="33" customHeight="1" spans="1:7">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18" t="s">
-        <v>51</v>
-      </c>
+      <c r="A17" s="16"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -1836,7 +1675,7 @@
       <c r="G17" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="15">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
@@ -1847,13 +1686,11 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
     <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B13:G14"/>
+    <mergeCell ref="B16:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>